<commit_message>
update laptop and migration switch
</commit_message>
<xml_diff>
--- a/public/sampleSW.xlsx
+++ b/public/sampleSW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPABIBNBX013\Documents\ICT Project Software\new-itportal\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0B792C4-0505-4401-9116-21D03F1A8BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D57E181-94A6-404D-BB8F-8319B139EB7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AA518A1B-D065-49A0-8AFF-0FB34B05899E}"/>
   </bookViews>
@@ -248,12 +248,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -262,11 +258,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
@@ -658,7 +656,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,383 +677,370 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="2"/>
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="2"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="2"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="2"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="2"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="2"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="2"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="2"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="2"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="2"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="2"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="4"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="6"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="4"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="4"/>
     </row>
     <row r="16" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="J16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="K16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L16" s="4" t="s">
+      <c r="L16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M16" s="7"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
         <v>1</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="J17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="K17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L17" s="5"/>
-      <c r="M17" s="7"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
         <v>2</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="H18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="I18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="J18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="K18" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L18" s="5" t="s">
+      <c r="L18" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
         <v>3</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="H19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="I19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="J19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="K19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="L19" s="3" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update import AP, Switch, and Wirelless add row and update view Ap page add button download import data format, and updtae routes web
</commit_message>
<xml_diff>
--- a/public/sampleSW.xlsx
+++ b/public/sampleSW.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPABIBNBX013\Documents\ICT Project Software\new-itportal\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPABIBNBX013\Documents\ICT Project Software\new-itportal-first\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D57E181-94A6-404D-BB8F-8319B139EB7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9A7D39-1525-4BF2-91B5-7491C4861A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AA518A1B-D065-49A0-8AFF-0FB34B05899E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>max_id</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Ex tyre</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -156,6 +159,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -163,6 +167,7 @@
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -656,7 +661,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,7 +971,9 @@
       <c r="K17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L17" s="3"/>
+      <c r="L17" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3">

</xml_diff>